<commit_message>
Popup handling edit invoice page
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/ManageInvoiceTestData.xlsx
+++ b/binaries/FCfiles/ManageInvoiceTestData.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="93">
   <si>
     <t>Additional Handling Required</t>
   </si>
@@ -301,6 +301,12 @@
   </si>
   <si>
     <t>58233443</t>
+  </si>
+  <si>
+    <t>11-25-2021</t>
+  </si>
+  <si>
+    <t>58285533</t>
   </si>
 </sst>
 </file>
@@ -331,7 +337,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="166">
+  <fills count="174">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1158,8 +1164,48 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="164">
+  <borders count="172">
     <border>
       <left/>
       <right/>
@@ -1760,6 +1806,34 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
@@ -1768,7 +1842,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="93">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
@@ -1859,7 +1933,11 @@
     <xf applyBorder="true" applyFill="true" borderId="157" fillId="159" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="159" fillId="161" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="161" fillId="163" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="165" borderId="163" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="163" fillId="165" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="165" fillId="167" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="167" fillId="169" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="169" fillId="171" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="173" borderId="171" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -2348,8 +2426,8 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="85" t="s">
-        <v>88</v>
+      <c r="A2" s="89" t="s">
+        <v>91</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
@@ -2363,7 +2441,7 @@
       <c r="E2" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="88" t="s">
+      <c r="F2" s="92" t="s">
         <v>54</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -2381,8 +2459,8 @@
       <c r="K2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="L2" s="87" t="s">
-        <v>90</v>
+      <c r="L2" s="91" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>